<commit_message>
simple logic between TR2 OPT and RA
</commit_message>
<xml_diff>
--- a/ra_exploer/examples/配向力_TR2_All.xlsx
+++ b/ra_exploer/examples/配向力_TR2_All.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\dimsp\Documents\Projects\td_toolkits_reconstruc\ra_exploer\examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A35823AE-4A4C-4802-8EE4-06FAEF52D14D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7BF3F84-4DAC-41D9-BDD8-D9A44AF42BF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="16440" windowHeight="28440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Δangle" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="22">
   <si>
     <t>Δangle</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -142,10 +142,6 @@
   </si>
   <si>
     <t>N.A.</t>
-  </si>
-  <si>
-    <t>T.B.D</t>
-    <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -608,10 +604,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K7"/>
+  <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19.5"/>
@@ -795,76 +791,6 @@
         <v>200320</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="21">
-      <c r="A6" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="B6" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E6" s="1">
-        <v>0.18</v>
-      </c>
-      <c r="F6" s="1">
-        <v>14</v>
-      </c>
-      <c r="G6" s="1">
-        <v>60</v>
-      </c>
-      <c r="H6" s="1">
-        <v>300</v>
-      </c>
-      <c r="I6" s="1">
-        <v>60</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="K6" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" ht="21">
-      <c r="A7" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="B7" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E7" s="1">
-        <v>0.08</v>
-      </c>
-      <c r="F7" s="1">
-        <v>14</v>
-      </c>
-      <c r="G7" s="1">
-        <v>60</v>
-      </c>
-      <c r="H7" s="1">
-        <v>300</v>
-      </c>
-      <c r="I7" s="1">
-        <v>60</v>
-      </c>
-      <c r="J7" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="K7" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>